<commit_message>
advt, presences, prices, stocks: assede [scratch] attribute.
</commit_message>
<xml_diff>
--- a/htdocs/assets/advt.xlsx
+++ b/htdocs/assets/advt.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -79,6 +79,9 @@
     <t xml:space="preserve">Руководитель</t>
   </si>
   <si>
+    <t xml:space="preserve">♺</t>
+  </si>
+  <si>
     <t xml:space="preserve">14</t>
   </si>
   <si>
@@ -89,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19</t>
   </si>
   <si>
     <t xml:space="preserve">20</t>
@@ -149,7 +155,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,6 +166,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF355C83"/>
         <bgColor rgb="FF666666"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9211E"/>
+        <bgColor rgb="FF993366"/>
       </patternFill>
     </fill>
   </fills>
@@ -212,7 +224,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -274,6 +286,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -348,7 +364,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF355C83"/>
       <rgbColor rgb="FF333333"/>
@@ -365,11 +381,11 @@
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -391,9 +407,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="25.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="5" width="11.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="3" width="19.65"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="61" min="20" style="6" width="8.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="62" style="7" width="8.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="4.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="60" min="21" style="6" width="8.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="61" style="7" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -415,6 +432,7 @@
       <c r="Q1" s="10"/>
       <c r="R1" s="11"/>
       <c r="S1" s="10"/>
+      <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
@@ -477,6 +495,9 @@
       <c r="S2" s="14" t="s">
         <v>18</v>
       </c>
+      <c r="T2" s="16" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="n">
@@ -488,53 +509,56 @@
       <c r="C3" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D3" s="16" t="n">
+      <c r="D3" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="E3" s="16" t="n">
+      <c r="E3" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="F3" s="16" t="n">
+      <c r="F3" s="17" t="n">
         <v>6</v>
       </c>
-      <c r="G3" s="16" t="n">
+      <c r="G3" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="H3" s="16" t="n">
+      <c r="H3" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="I3" s="16" t="n">
+      <c r="I3" s="17" t="n">
         <v>9</v>
       </c>
-      <c r="J3" s="16" t="n">
+      <c r="J3" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="K3" s="16" t="n">
+      <c r="K3" s="17" t="n">
         <v>11</v>
       </c>
-      <c r="L3" s="16" t="n">
+      <c r="L3" s="17" t="n">
         <v>12</v>
       </c>
-      <c r="M3" s="16" t="n">
+      <c r="M3" s="17" t="n">
         <v>13</v>
       </c>
-      <c r="N3" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" s="16" t="s">
+      <c r="N3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="O3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="P3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="17" t="n">
-        <v>19</v>
-      </c>
-      <c r="S3" s="16" t="s">
+      <c r="Q3" s="17" t="s">
         <v>23</v>
+      </c>
+      <c r="R3" s="18" t="n">
+        <v>18</v>
+      </c>
+      <c r="S3" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3" s="16" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
*: fixed xlsx templates.
</commit_message>
<xml_diff>
--- a/htdocs/assets/advt.xlsx
+++ b/htdocs/assets/advt.xlsx
@@ -106,11 +106,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -141,13 +141,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="7"/>
-      <color rgb="FF666666"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FFFFFFFF"/>
       <name val="Verdana"/>
@@ -165,7 +158,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF355C83"/>
-        <bgColor rgb="FF666666"/>
+        <bgColor rgb="FF333399"/>
       </patternFill>
     </fill>
     <fill>
@@ -224,7 +217,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -257,47 +250,31 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -358,7 +335,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666666"/>
+      <rgbColor rgb="FF355C83"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -366,7 +343,7 @@
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF355C83"/>
+      <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
@@ -374,18 +351,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ3"/>
+  <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -410,161 +387,138 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="4.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="60" min="21" style="6" width="8.5"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="61" style="7" width="8.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="10.5"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="10"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
+    <row r="1" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="13" t="s">
+    <row r="2" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="D2" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="F2" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="G2" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="H2" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="I2" s="13" t="n">
         <v>9</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="J2" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="K2" s="13" t="n">
         <v>11</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="L2" s="13" t="n">
         <v>12</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="M2" s="13" t="n">
         <v>13</v>
       </c>
-      <c r="O2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="S2" s="14" t="s">
+      <c r="N2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="14" t="n">
         <v>18</v>
       </c>
-      <c r="T2" s="16" t="s">
-        <v>19</v>
+      <c r="S2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="15" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" s="17" t="n">
-        <v>4</v>
-      </c>
-      <c r="E3" s="17" t="n">
-        <v>5</v>
-      </c>
-      <c r="F3" s="17" t="n">
-        <v>6</v>
-      </c>
-      <c r="G3" s="17" t="n">
-        <v>7</v>
-      </c>
-      <c r="H3" s="17" t="n">
-        <v>8</v>
-      </c>
-      <c r="I3" s="17" t="n">
-        <v>9</v>
-      </c>
-      <c r="J3" s="17" t="n">
-        <v>10</v>
-      </c>
-      <c r="K3" s="17" t="n">
-        <v>11</v>
-      </c>
-      <c r="L3" s="17" t="n">
-        <v>12</v>
-      </c>
-      <c r="M3" s="17" t="n">
-        <v>13</v>
-      </c>
-      <c r="N3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" s="18" t="n">
-        <v>18</v>
-      </c>
-      <c r="S3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="T3" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>